<commit_message>
Fix choice name REGEX and associated test
</commit_message>
<xml_diff>
--- a/qtools2/test/forms/nonascii1.xlsx
+++ b/qtools2/test/forms/nonascii1.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>type</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t xml:space="preserve">wer asd w </t>
+  </si>
+  <si>
+    <t>skipped</t>
   </si>
 </sst>
 </file>
@@ -187,9 +190,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -696,10 +700,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -727,6 +731,14 @@
     <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="2"/>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>